<commit_message>
Functional ecology review Updated scripts adn results Answer to reviewers and revised main documents
</commit_message>
<xml_diff>
--- a/results/supplementary/Table 3. Germination glm results.xlsx
+++ b/results/supplementary/Table 3. Germination glm results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\Hidro_thermal_experiments\results\supplementary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Dianthus_PEG/results/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_40DAF4AD6E27153BFC008EC9A6994590F49CDDCE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB6A91C1-C12C-4B22-9C42-3C0FC40A897E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Model formula specification</t>
   </si>
@@ -55,9 +56,6 @@
     <t>storage treatment</t>
   </si>
   <si>
-    <t>Both storage treatments considered</t>
-  </si>
-  <si>
     <t>WP treatment</t>
   </si>
   <si>
@@ -68,13 +66,25 @@
   </si>
   <si>
     <t xml:space="preserve"> cbind(germinated, viable - germinated) ~ WP_treatment * storage treatment + (1 | summit/ID) Family: binomial (logit)</t>
+  </si>
+  <si>
+    <t>Both storage treatments considered (n= 24)</t>
+  </si>
+  <si>
+    <t>Both storage treatments considered (n= 12)</t>
+  </si>
+  <si>
+    <t>Full dataset</t>
+  </si>
+  <si>
+    <t>Subset only with subpopulations  in both storage treatments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +95,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -111,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -120,6 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,10 +154,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,130 +472,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.75" customWidth="1"/>
-    <col min="2" max="2" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="C4">
         <v>2.8083399999999998</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>7.2650000000000006E-2</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>38.659999999999997</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2"/>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>-0.42902000000000001</v>
-      </c>
-      <c r="D4">
-        <v>4.428E-2</v>
-      </c>
-      <c r="E4">
-        <v>-9.69</v>
-      </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>-0.42902000000000001</v>
+      </c>
+      <c r="D5">
+        <v>4.428E-2</v>
+      </c>
+      <c r="E5">
+        <v>-9.69</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>0.97418000000000005</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>0.12614</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>7.72</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>1.1400000000000001E-14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>7.5509000000000004</v>
+      </c>
+      <c r="D9">
+        <v>0.26279999999999998</v>
+      </c>
+      <c r="E9">
+        <v>28.734999999999999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>-2.4691000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="E10">
+        <v>-17.091999999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>-2.1598999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.32829999999999998</v>
+      </c>
+      <c r="E11">
+        <v>-6.5789999999999997</v>
+      </c>
+      <c r="F11">
+        <v>4.7200000000000002E-11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>